<commit_message>
Baseline for VGA functionality.
</commit_message>
<xml_diff>
--- a/hardware/kicad/6502/6502-BOM.xlsx
+++ b/hardware/kicad/6502/6502-BOM.xlsx
@@ -37,7 +37,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, </t>
+    <t>C1</t>
   </si>
   <si>
     <t>1µF</t>
@@ -55,7 +55,7 @@
     <t>Unpolarized capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C2, C3, C4, C5, C6, C7, C8, C9, C10, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, </t>
+    <t>C2, C3, C4, C5, C6, C7, C8, C9, C10, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23</t>
   </si>
   <si>
     <t>0.1µF</t>
@@ -67,7 +67,7 @@
     <t>Capacitor_THT:C_Disc_D5.0mm_W2.5mm_P2.50mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C11, </t>
+    <t>C11</t>
   </si>
   <si>
     <t>33pF</t>
@@ -79,7 +79,7 @@
     <t>Capacitor_THT:C_Disc_D5.0mm_W2.5mm_P5.00mm</t>
   </si>
   <si>
-    <t xml:space="preserve">D1, </t>
+    <t>D1</t>
   </si>
   <si>
     <t>1N5819</t>
@@ -94,7 +94,7 @@
     <t>40V 1A Schottky Barrier Rectifier Diode, DO-41</t>
   </si>
   <si>
-    <t xml:space="preserve">D2, </t>
+    <t>D2</t>
   </si>
   <si>
     <t>LED</t>
@@ -106,7 +106,7 @@
     <t>Light emitting diode</t>
   </si>
   <si>
-    <t xml:space="preserve">J1, </t>
+    <t>J1</t>
   </si>
   <si>
     <t>Barrel_Jack</t>
@@ -121,7 +121,7 @@
     <t>DC Barrel Jack</t>
   </si>
   <si>
-    <t xml:space="preserve">J2, </t>
+    <t>J2</t>
   </si>
   <si>
     <t>Bus_Header</t>
@@ -139,7 +139,7 @@
     <t>Generic connector, double row, 02x20, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers)</t>
   </si>
   <si>
-    <t xml:space="preserve">J3, </t>
+    <t>J3</t>
   </si>
   <si>
     <t>LCD_Header</t>
@@ -157,7 +157,7 @@
     <t>Generic connector, single row, 01x16</t>
   </si>
   <si>
-    <t xml:space="preserve">J4, </t>
+    <t>J4</t>
   </si>
   <si>
     <t>UART_Header</t>
@@ -175,13 +175,13 @@
     <t>Generic connector, single row, 01x06</t>
   </si>
   <si>
-    <t xml:space="preserve">J5, </t>
+    <t>J5</t>
   </si>
   <si>
     <t>VIA_Header</t>
   </si>
   <si>
-    <t xml:space="preserve">J6, </t>
+    <t>J6</t>
   </si>
   <si>
     <t>VGA_Out</t>
@@ -199,7 +199,7 @@
     <t>15-pin female D-SUB connector, High density (3 columns), Triple Row, Generic, VGA-connector</t>
   </si>
   <si>
-    <t xml:space="preserve">J7, </t>
+    <t>J7</t>
   </si>
   <si>
     <t>GAL_Header</t>
@@ -208,7 +208,7 @@
     <t>https://mou.sr/3QNGOmm</t>
   </si>
   <si>
-    <t xml:space="preserve">J8, </t>
+    <t>J8</t>
   </si>
   <si>
     <t>VGA_Address_Header</t>
@@ -217,7 +217,7 @@
     <t>Generic connector, double row, 02x20</t>
   </si>
   <si>
-    <t xml:space="preserve">J9, </t>
+    <t>J9</t>
   </si>
   <si>
     <t>VGA_Clock</t>
@@ -235,7 +235,7 @@
     <t>Generic connector, double row, 02x03</t>
   </si>
   <si>
-    <t xml:space="preserve">J10, </t>
+    <t>J10</t>
   </si>
   <si>
     <t>VGA_Data_Header</t>
@@ -253,7 +253,7 @@
     <t>Generic connector, double row, 02x08, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers)</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R2, R3, R4, R5, R6, R13, R14, R15, R16, </t>
+    <t>R1, R2, R3, R4, R5, R6, R13, R14, R15, R16</t>
   </si>
   <si>
     <t>1k</t>
@@ -271,13 +271,13 @@
     <t>Resistor, US symbol</t>
   </si>
   <si>
-    <t xml:space="preserve">R7, R9, R11, </t>
+    <t>R7, R9, R11</t>
   </si>
   <si>
     <t>https://mou.sr/3qEoBgq</t>
   </si>
   <si>
-    <t xml:space="preserve">R8, R10, R12, </t>
+    <t>R8, R10, R12</t>
   </si>
   <si>
     <t>1.5k</t>
@@ -286,7 +286,7 @@
     <t>https://mou.sr/3qJ1EZL</t>
   </si>
   <si>
-    <t xml:space="preserve">RV1, </t>
+    <t>RV1</t>
   </si>
   <si>
     <t>R_Potentiometer</t>
@@ -301,7 +301,7 @@
     <t>Potentiometer</t>
   </si>
   <si>
-    <t xml:space="preserve">SW1, SW2, SW3, SW4, SW5, </t>
+    <t>SW1, SW2, SW3, SW4, SW5</t>
   </si>
   <si>
     <t>SW_Push</t>
@@ -316,7 +316,7 @@
     <t>Push button switch, generic, two pins</t>
   </si>
   <si>
-    <t xml:space="preserve">SW6, </t>
+    <t>SW6</t>
   </si>
   <si>
     <t>SW_VGA_CLOCK</t>
@@ -334,7 +334,7 @@
     <t>Switch, single pole double throw</t>
   </si>
   <si>
-    <t xml:space="preserve">SW7, </t>
+    <t>SW7</t>
   </si>
   <si>
     <t>DMA_DIP</t>
@@ -352,10 +352,10 @@
     <t>4x DIP Switch, Single Pole Single Throw (SPST) switch, small symbol</t>
   </si>
   <si>
-    <t xml:space="preserve">SW8, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1, U7, U9, U12, </t>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>U1, U7, U9, U12</t>
   </si>
   <si>
     <t>GAL16V8</t>
@@ -373,7 +373,7 @@
     <t>Programmable Logic Array, DIP-20/SOIC-20/PLCC-20</t>
   </si>
   <si>
-    <t xml:space="preserve">U2, </t>
+    <t>U2</t>
   </si>
   <si>
     <t>W65C02SxP</t>
@@ -391,7 +391,7 @@
     <t>W65C02S 8-bit CMOS General Purpose Microprocessor, DIP-40</t>
   </si>
   <si>
-    <t xml:space="preserve">U3, </t>
+    <t>U3</t>
   </si>
   <si>
     <t>28C256</t>
@@ -409,7 +409,7 @@
     <t>Paged Parallel EEPROM 256Kb (32K x 8), DIP-28/SOIC-28</t>
   </si>
   <si>
-    <t xml:space="preserve">U4, </t>
+    <t>U4</t>
   </si>
   <si>
     <t>HM62256BLP</t>
@@ -424,7 +424,7 @@
     <t>32,768-word Ã— 8-bit High Speed CMOS Static RAM, 70ns, DIP-28</t>
   </si>
   <si>
-    <t xml:space="preserve">U5, </t>
+    <t>U5</t>
   </si>
   <si>
     <t>W65C22SxP</t>
@@ -436,7 +436,7 @@
     <t>W65C22S CMOS Versatile Interface Adapter (VIA), 20-pin I/O, 2 Timer/Counters, DIP-40</t>
   </si>
   <si>
-    <t xml:space="preserve">U6, U11, U18, U19, U20, U21, </t>
+    <t>U6, U11, U18, U19, U20, U21</t>
   </si>
   <si>
     <t>74LS161</t>
@@ -454,7 +454,7 @@
     <t>Synchronous 4-bit programmable binary Counter</t>
   </si>
   <si>
-    <t xml:space="preserve">U8, </t>
+    <t>U8</t>
   </si>
   <si>
     <t>W65C51NxP</t>
@@ -466,7 +466,7 @@
     <t>W65C51N CMOS Asynchronous Communication Interface Adapter (ACIA), Serial UART, DIP-28</t>
   </si>
   <si>
-    <t xml:space="preserve">U10, U13, </t>
+    <t>U10, U13</t>
   </si>
   <si>
     <t>74HC00</t>
@@ -484,7 +484,7 @@
     <t>quad 2-input NAND gate</t>
   </si>
   <si>
-    <t xml:space="preserve">U14, </t>
+    <t>U14</t>
   </si>
   <si>
     <t>74HC74</t>
@@ -496,7 +496,7 @@
     <t>Dual D Flip-flop, Set &amp; Reset</t>
   </si>
   <si>
-    <t xml:space="preserve">U15, U16, U17, </t>
+    <t>U15, U16, U17</t>
   </si>
   <si>
     <t>74HC245</t>
@@ -508,7 +508,7 @@
     <t>Octal BUS Transceivers, 3-State outputs</t>
   </si>
   <si>
-    <t xml:space="preserve">X1, X2, X4, </t>
+    <t>X1, X2, X4</t>
   </si>
   <si>
     <t>TFT680</t>
@@ -526,7 +526,7 @@
     <t>Crystal Clock Oscillator, DIP14-style metal package</t>
   </si>
   <si>
-    <t xml:space="preserve">X3, </t>
+    <t>X3</t>
   </si>
   <si>
     <t>TFT660</t>

</xml_diff>